<commit_message>
pokus with commit... still no idea how it works...
</commit_message>
<xml_diff>
--- a/kliceni_data.xlsx
+++ b/kliceni_data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -10,12 +10,12 @@
     <sheet name="kliceni" sheetId="1" r:id="rId1"/>
     <sheet name="proklicovani" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>no1</t>
   </si>
@@ -138,13 +138,16 @@
   </si>
   <si>
     <t>cm5</t>
+  </si>
+  <si>
+    <t>total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,12 +176,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -194,7 +198,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv sady Office">
   <a:themeElements>
     <a:clrScheme name="Kancelář">
       <a:dk1>
@@ -236,7 +240,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kancelář">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -268,10 +272,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -303,7 +306,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kancelář">
@@ -479,16 +481,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18">
       <c r="B1" s="1">
         <v>42016</v>
       </c>
@@ -541,7 +543,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -598,7 +600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -655,7 +657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -712,7 +714,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -769,7 +771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -826,7 +828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -883,7 +885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -940,7 +942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -997,7 +999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1054,7 +1056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1111,7 +1113,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1168,7 +1170,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1225,7 +1227,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1282,7 +1284,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1339,7 +1341,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1396,7 +1398,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1453,7 +1455,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1510,7 +1512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1567,7 +1569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -1624,7 +1626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1681,7 +1683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -1738,7 +1740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -1801,16 +1803,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21">
       <c r="B1" s="1">
         <v>42016</v>
       </c>
@@ -1865,8 +1867,11 @@
       <c r="S1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1926,8 +1931,15 @@
         <f>25-R2</f>
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T2">
+        <v>25</v>
+      </c>
+      <c r="U2">
+        <f>R2/T2</f>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1987,8 +1999,15 @@
         <f t="shared" ref="S3:S13" si="1">25-R3</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T3">
+        <v>25</v>
+      </c>
+      <c r="U3">
+        <f t="shared" ref="U3:U13" si="2">R3/T3</f>
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -2048,8 +2067,15 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T4">
+        <v>25</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="2"/>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -2109,8 +2135,15 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T5">
+        <v>25</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="2"/>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -2170,8 +2203,15 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T6">
+        <v>25</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -2231,8 +2271,15 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T7">
+        <v>25</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="2"/>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -2292,8 +2339,15 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T8">
+        <v>25</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -2353,8 +2407,15 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T9">
+        <v>25</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -2414,8 +2475,15 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T10">
+        <v>25</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -2475,8 +2543,15 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T11">
+        <v>25</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -2536,8 +2611,15 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T12">
+        <v>25</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -2597,8 +2679,18 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="T13">
+        <v>25</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="8:13">
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="8:13">
       <c r="H19" t="s">
         <v>37</v>
       </c>
@@ -2610,8 +2702,15 @@
         <f>S2+S3+S4</f>
         <v>65</v>
       </c>
-    </row>
-    <row r="20" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="K19">
+        <v>75</v>
+      </c>
+      <c r="L19">
+        <f>I19/K19</f>
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="20" spans="8:13">
       <c r="H20" t="s">
         <v>38</v>
       </c>
@@ -2623,8 +2722,15 @@
         <f>SUM(S5:S7)</f>
         <v>68</v>
       </c>
-    </row>
-    <row r="21" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="K20">
+        <v>75</v>
+      </c>
+      <c r="L20">
+        <f t="shared" ref="L20:L22" si="3">I20/K20</f>
+        <v>9.3333333333333338E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="8:13">
       <c r="H21" t="s">
         <v>39</v>
       </c>
@@ -2635,8 +2741,15 @@
       <c r="J21">
         <v>75</v>
       </c>
-    </row>
-    <row r="22" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <v>75</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="8:13">
       <c r="H22" t="s">
         <v>40</v>
       </c>
@@ -2646,8 +2759,16 @@
       <c r="J22">
         <v>75</v>
       </c>
+      <c r="K22">
+        <v>75</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added some calculations withing the tables and raw data
</commit_message>
<xml_diff>
--- a/kliceni_data.xlsx
+++ b/kliceni_data.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="kliceni" sheetId="1" r:id="rId1"/>
     <sheet name="proklicovani" sheetId="2" r:id="rId2"/>
+    <sheet name="List1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
   <si>
     <t>no1</t>
   </si>
@@ -141,6 +142,42 @@
   </si>
   <si>
     <t>total</t>
+  </si>
+  <si>
+    <t>1cm</t>
+  </si>
+  <si>
+    <t>3cm</t>
+  </si>
+  <si>
+    <t>5cm</t>
+  </si>
+  <si>
+    <t>laborka</t>
+  </si>
+  <si>
+    <t>venku</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>germ</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>exp</t>
+  </si>
+  <si>
+    <t>treatment</t>
+  </si>
+  <si>
+    <t>lab</t>
+  </si>
+  <si>
+    <t>ext</t>
   </si>
 </sst>
 </file>
@@ -1804,10 +1841,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U22"/>
+  <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView topLeftCell="C12" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19:L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2687,10 +2724,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="8:13">
+    <row r="18" spans="6:13">
+      <c r="L18" t="s">
+        <v>47</v>
+      </c>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="8:13">
+    <row r="19" spans="6:13">
+      <c r="F19" t="s">
+        <v>45</v>
+      </c>
       <c r="H19" t="s">
         <v>37</v>
       </c>
@@ -2710,7 +2753,7 @@
         <v>0.13333333333333333</v>
       </c>
     </row>
-    <row r="20" spans="8:13">
+    <row r="20" spans="6:13">
       <c r="H20" t="s">
         <v>38</v>
       </c>
@@ -2730,7 +2773,7 @@
         <v>9.3333333333333338E-2</v>
       </c>
     </row>
-    <row r="21" spans="8:13">
+    <row r="21" spans="6:13">
       <c r="H21" t="s">
         <v>39</v>
       </c>
@@ -2749,7 +2792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="8:13">
+    <row r="22" spans="6:13">
       <c r="H22" t="s">
         <v>40</v>
       </c>
@@ -2764,6 +2807,165 @@
       </c>
       <c r="L22">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="6:13">
+      <c r="F25" t="s">
+        <v>46</v>
+      </c>
+      <c r="H25" t="s">
+        <v>37</v>
+      </c>
+      <c r="I25">
+        <v>40</v>
+      </c>
+      <c r="J25">
+        <v>35</v>
+      </c>
+      <c r="K25">
+        <v>75</v>
+      </c>
+      <c r="L25">
+        <f>I25/K25</f>
+        <v>0.53333333333333333</v>
+      </c>
+    </row>
+    <row r="26" spans="6:13">
+      <c r="H26" t="s">
+        <v>42</v>
+      </c>
+      <c r="I26">
+        <v>26</v>
+      </c>
+      <c r="J26">
+        <v>49</v>
+      </c>
+      <c r="K26">
+        <v>75</v>
+      </c>
+      <c r="L26">
+        <f t="shared" ref="L26:L28" si="4">I26/K26</f>
+        <v>0.34666666666666668</v>
+      </c>
+    </row>
+    <row r="27" spans="6:13">
+      <c r="H27" t="s">
+        <v>43</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>75</v>
+      </c>
+      <c r="K27">
+        <v>75</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="6:13">
+      <c r="H28" t="s">
+        <v>44</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>75</v>
+      </c>
+      <c r="K28">
+        <v>75</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="6:13">
+      <c r="H32" t="s">
+        <v>37</v>
+      </c>
+      <c r="I32">
+        <f>I19+I25</f>
+        <v>50</v>
+      </c>
+      <c r="J32">
+        <f t="shared" ref="J32:K32" si="5">J19+J25</f>
+        <v>100</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="5"/>
+        <v>150</v>
+      </c>
+      <c r="L32">
+        <f>I32/K32</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="33" spans="8:12">
+      <c r="H33" t="s">
+        <v>42</v>
+      </c>
+      <c r="I33">
+        <f t="shared" ref="I33:K35" si="6">I20+I26</f>
+        <v>33</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="6"/>
+        <v>117</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="6"/>
+        <v>150</v>
+      </c>
+      <c r="L33">
+        <f t="shared" ref="L33:L35" si="7">I33/K33</f>
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="34" spans="8:12">
+      <c r="H34" t="s">
+        <v>43</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="6"/>
+        <v>150</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="6"/>
+        <v>150</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="8:12">
+      <c r="H35" t="s">
+        <v>44</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="6"/>
+        <v>150</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="6"/>
+        <v>150</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -2771,4 +2973,143 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>75</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>75</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>75</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>75</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>75</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>